<commit_message>
Updated Sprint backlog Day 1
Added some extra tasks and updated for day 1
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Agile Sprint Backlog-sprint 2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Agile Sprint Backlog-sprint 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\agile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\Team-16-agile\Sprint 2\Sprint_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576AE7A-78DA-4FE8-9507-C7994C4B9206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0BDDE4-276E-4D4F-ACEE-936C2A802193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$V$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Sprint 1 - Day 1'!$B$2:$U$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Sprint 2 - Day 1'!$B$2:$U$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Sprint 2 - Day 1'!$B$2:$U$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="61">
   <si>
     <t>User Story #1</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Everyone</t>
   </si>
   <si>
-    <t xml:space="preserve">Website accessibilty </t>
-  </si>
-  <si>
     <t>Sprint retrospective</t>
   </si>
   <si>
@@ -208,6 +205,21 @@
   </si>
   <si>
     <t>Users should be able to input their location manually</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Connecting Backend to the frontend</t>
+  </si>
+  <si>
+    <t>Conecting the search bar with back end to give the functionality of search</t>
+  </si>
+  <si>
+    <t>Connecting the result cards with the backend</t>
+  </si>
+  <si>
+    <t>Connecting filters</t>
   </si>
 </sst>
 </file>
@@ -349,12 +361,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,15 +906,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2 - Day 1'!$F$18:$K$18</c:f>
+              <c:f>'Sprint 2 - Day 1'!$F$21:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1121,7 +1133,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>431800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1504,29 +1516,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -5527,28 +5539,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
@@ -9238,11 +9250,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AA113"/>
+  <dimension ref="B1:AA116"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G17"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9263,28 +9275,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
@@ -9342,7 +9354,7 @@
     </row>
     <row r="3" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
@@ -9370,21 +9382,23 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="9">
         <v>5</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -9406,9 +9420,9 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
@@ -9420,7 +9434,9 @@
       <c r="F5" s="9">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9">
+        <v>6</v>
+      </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -9444,7 +9460,7 @@
     </row>
     <row r="6" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
@@ -9456,7 +9472,9 @@
       <c r="F6" s="9">
         <v>5</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>5</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -9478,21 +9496,23 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
     </row>
-    <row r="7" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="9">
         <v>10</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9">
+        <v>4</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -9515,24 +9535,18 @@
       <c r="AA7" s="4"/>
     </row>
     <row r="8" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="9">
-        <v>5</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -9551,18 +9565,26 @@
       <c r="AA8" s="4"/>
     </row>
     <row r="9" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9">
+        <v>10</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -9592,9 +9614,11 @@
         <v>38</v>
       </c>
       <c r="F10" s="9">
-        <v>10</v>
-      </c>
-      <c r="G10" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -9616,20 +9640,16 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
     </row>
-    <row r="11" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="9">
-        <v>5</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -9652,17 +9672,23 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
     </row>
-    <row r="12" spans="2:27" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="E12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="9">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9">
+        <v>6</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -9686,7 +9712,7 @@
     </row>
     <row r="13" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
@@ -9696,9 +9722,11 @@
         <v>38</v>
       </c>
       <c r="F13" s="9">
-        <v>7</v>
-      </c>
-      <c r="G13" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -9721,24 +9749,18 @@
       <c r="AA13" s="4"/>
     </row>
     <row r="14" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="9">
-        <v>3</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+      <c r="B14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -9756,19 +9778,27 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
     </row>
-    <row r="15" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+    <row r="15" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="9">
+        <v>5</v>
+      </c>
+      <c r="G15" s="9">
+        <v>5</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -9786,21 +9816,23 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="9">
-        <v>10</v>
-      </c>
-      <c r="G16" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="G16" s="9">
+        <v>4</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -9822,73 +9854,55 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="2:27" s="12" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F17" s="9">
-        <v>5</v>
-      </c>
-      <c r="G17" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="G17" s="9">
+        <v>8</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-    </row>
-    <row r="18" spans="2:27" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
-        <f>SUM(F3:F17)</f>
-        <v>71</v>
-      </c>
-      <c r="G18" s="5">
-        <f>SUM(G3:G17)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <f>SUM(H3:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <f>SUM(I3:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <f>SUM(J3:J17)</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <f>SUM(K3:K17)</f>
-        <v>0</v>
-      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+    </row>
+    <row r="18" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -9906,17 +9920,27 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
     </row>
-    <row r="19" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+    <row r="19" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="9">
+        <v>10</v>
+      </c>
+      <c r="G19" s="9">
+        <v>7</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -9934,45 +9958,75 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+    <row r="20" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+    </row>
+    <row r="21" spans="2:27" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5">
+        <f t="shared" ref="F21:K21" si="0">SUM(F3:F20)</f>
+        <v>83</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -9990,7 +10044,7 @@
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="1"/>
       <c r="D22" s="4"/>
@@ -12566,6 +12620,90 @@
       <c r="Z113" s="4"/>
       <c r="AA113" s="4"/>
     </row>
+    <row r="114" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4"/>
+      <c r="W114" s="4"/>
+      <c r="X114" s="4"/>
+      <c r="Y114" s="4"/>
+      <c r="Z114" s="4"/>
+      <c r="AA114" s="4"/>
+    </row>
+    <row r="115" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="4"/>
+      <c r="W115" s="4"/>
+      <c r="X115" s="4"/>
+      <c r="Y115" s="4"/>
+      <c r="Z115" s="4"/>
+      <c r="AA115" s="4"/>
+    </row>
+    <row r="116" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="4"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+      <c r="U116" s="4"/>
+      <c r="V116" s="4"/>
+      <c r="W116" s="4"/>
+      <c r="X116" s="4"/>
+      <c r="Y116" s="4"/>
+      <c r="Z116" s="4"/>
+      <c r="AA116" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:U1"/>
@@ -12577,15 +12715,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB9990FB49C9134A850E6553B234458F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95d3b0f826e3528efb1f5f47bd4e34cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="93e1a4ff-8964-4a69-82aa-a6ae8e76f3bb" xmlns:ns4="ef82ad94-d9c5-4f1c-80c3-e3984065e9aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c95535c12b49328303a3e4b018f1ea58" ns3:_="" ns4:_="">
     <xsd:import namespace="93e1a4ff-8964-4a69-82aa-a6ae8e76f3bb"/>
@@ -12794,6 +12923,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -12801,14 +12939,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF8BB5BC-83A8-4EE2-A3A8-C39502C9DC55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64135FEA-1EDF-42A1-9BA1-AA1C06030FAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12823,6 +12953,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF8BB5BC-83A8-4EE2-A3A8-C39502C9DC55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Sprint backlog for day 5 completed
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Agile Sprint Backlog-sprint 2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Agile Sprint Backlog-sprint 2.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6BFB12-7E27-4803-893B-B6B373EAC2A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311A7F35-E40E-43FC-9871-4EBBE70FAC57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2 - Day 1" sheetId="12" r:id="rId1"/>
     <sheet name="Sprint 2 - Day 2" sheetId="13" r:id="rId2"/>
     <sheet name="Sprint 2 - Day 3" sheetId="14" r:id="rId3"/>
     <sheet name="Sprint 2 - Day 4" sheetId="15" r:id="rId4"/>
+    <sheet name="Sprint 2 - Day 5" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint 2 - Day 1'!$B$2:$U$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Sprint 2 - Day 2'!$B$2:$U$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Sprint 2 - Day 3'!$B$2:$U$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Sprint 2 - Day 4'!$B$2:$U$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Sprint 2 - Day 5'!$B$2:$U$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="45">
   <si>
     <t>BACKLOG TASK &amp; ID</t>
   </si>
@@ -1196,6 +1198,219 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>SPRINT BURNDOWN</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sprint Burndown Chart</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2 - Day 5'!$G$2:$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>DAY 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DAY 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DAY 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DAY 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DAY 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 - Day 5'!$F$25:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6672-459C-873B-5A297A73E27B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2090279592"/>
+        <c:axId val="-2090276584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2090279592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090276584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090276584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090279592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="E5EEF6"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="9000000" scaled="0"/>
+        </a:gradFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="114300" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+        <a:schemeClr val="bg1">
+          <a:lumMod val="75000"/>
+          <a:alpha val="40000"/>
+        </a:schemeClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1346,6 +1561,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD672A08-4D78-4C0D-A4F6-0ABFED5CD4B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>431800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E774728-52CA-44D2-80F8-A539E4B31D15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12392,9 +12650,9 @@
   </sheetPr>
   <dimension ref="B1:AA120"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13357,7 +13615,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F24" s="9">
         <v>2</v>
@@ -13422,6 +13680,3766 @@
       <c r="K25" s="5">
         <f t="shared" ref="F25:K25" si="0">SUM(K3:K23)</f>
         <v>0</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+    </row>
+    <row r="26" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+    </row>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+    </row>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+    </row>
+    <row r="49" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+    </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+    </row>
+    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+    </row>
+    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+    </row>
+    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4"/>
+    </row>
+    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+    </row>
+    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+    </row>
+    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+    </row>
+    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
+      <c r="AA59" s="4"/>
+    </row>
+    <row r="60" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
+      <c r="AA60" s="4"/>
+    </row>
+    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="4"/>
+      <c r="AA61" s="4"/>
+    </row>
+    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="4"/>
+      <c r="AA62" s="4"/>
+    </row>
+    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="4"/>
+      <c r="AA63" s="4"/>
+    </row>
+    <row r="64" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="4"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+      <c r="Z64" s="4"/>
+      <c r="AA64" s="4"/>
+    </row>
+    <row r="65" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="4"/>
+      <c r="W65" s="4"/>
+      <c r="X65" s="4"/>
+      <c r="Y65" s="4"/>
+      <c r="Z65" s="4"/>
+      <c r="AA65" s="4"/>
+    </row>
+    <row r="66" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+      <c r="U66" s="4"/>
+      <c r="V66" s="4"/>
+      <c r="W66" s="4"/>
+      <c r="X66" s="4"/>
+      <c r="Y66" s="4"/>
+      <c r="Z66" s="4"/>
+      <c r="AA66" s="4"/>
+    </row>
+    <row r="67" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
+      <c r="X67" s="4"/>
+      <c r="Y67" s="4"/>
+      <c r="Z67" s="4"/>
+      <c r="AA67" s="4"/>
+    </row>
+    <row r="68" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+      <c r="U68" s="4"/>
+      <c r="V68" s="4"/>
+      <c r="W68" s="4"/>
+      <c r="X68" s="4"/>
+      <c r="Y68" s="4"/>
+      <c r="Z68" s="4"/>
+      <c r="AA68" s="4"/>
+    </row>
+    <row r="69" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="4"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4"/>
+      <c r="Z69" s="4"/>
+      <c r="AA69" s="4"/>
+    </row>
+    <row r="70" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="4"/>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
+      <c r="Y70" s="4"/>
+      <c r="Z70" s="4"/>
+      <c r="AA70" s="4"/>
+    </row>
+    <row r="71" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
+      <c r="Y71" s="4"/>
+      <c r="Z71" s="4"/>
+      <c r="AA71" s="4"/>
+    </row>
+    <row r="72" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="4"/>
+      <c r="AA72" s="4"/>
+    </row>
+    <row r="73" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="4"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="4"/>
+      <c r="Z73" s="4"/>
+      <c r="AA73" s="4"/>
+    </row>
+    <row r="74" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="4"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="4"/>
+      <c r="U74" s="4"/>
+      <c r="V74" s="4"/>
+      <c r="W74" s="4"/>
+      <c r="X74" s="4"/>
+      <c r="Y74" s="4"/>
+      <c r="Z74" s="4"/>
+      <c r="AA74" s="4"/>
+    </row>
+    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="4"/>
+      <c r="U75" s="4"/>
+      <c r="V75" s="4"/>
+      <c r="W75" s="4"/>
+      <c r="X75" s="4"/>
+      <c r="Y75" s="4"/>
+      <c r="Z75" s="4"/>
+      <c r="AA75" s="4"/>
+    </row>
+    <row r="76" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="4"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="4"/>
+      <c r="U76" s="4"/>
+      <c r="V76" s="4"/>
+      <c r="W76" s="4"/>
+      <c r="X76" s="4"/>
+      <c r="Y76" s="4"/>
+      <c r="Z76" s="4"/>
+      <c r="AA76" s="4"/>
+    </row>
+    <row r="77" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
+      <c r="X77" s="4"/>
+      <c r="Y77" s="4"/>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4"/>
+    </row>
+    <row r="78" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="4"/>
+      <c r="W78" s="4"/>
+      <c r="X78" s="4"/>
+      <c r="Y78" s="4"/>
+      <c r="Z78" s="4"/>
+      <c r="AA78" s="4"/>
+    </row>
+    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="4"/>
+      <c r="V79" s="4"/>
+      <c r="W79" s="4"/>
+      <c r="X79" s="4"/>
+      <c r="Y79" s="4"/>
+      <c r="Z79" s="4"/>
+      <c r="AA79" s="4"/>
+    </row>
+    <row r="80" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
+      <c r="X80" s="4"/>
+      <c r="Y80" s="4"/>
+      <c r="Z80" s="4"/>
+      <c r="AA80" s="4"/>
+    </row>
+    <row r="81" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+      <c r="U81" s="4"/>
+      <c r="V81" s="4"/>
+      <c r="W81" s="4"/>
+      <c r="X81" s="4"/>
+      <c r="Y81" s="4"/>
+      <c r="Z81" s="4"/>
+      <c r="AA81" s="4"/>
+    </row>
+    <row r="82" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="4"/>
+      <c r="S82" s="4"/>
+      <c r="T82" s="4"/>
+      <c r="U82" s="4"/>
+      <c r="V82" s="4"/>
+      <c r="W82" s="4"/>
+      <c r="X82" s="4"/>
+      <c r="Y82" s="4"/>
+      <c r="Z82" s="4"/>
+      <c r="AA82" s="4"/>
+    </row>
+    <row r="83" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="4"/>
+      <c r="S83" s="4"/>
+      <c r="T83" s="4"/>
+      <c r="U83" s="4"/>
+      <c r="V83" s="4"/>
+      <c r="W83" s="4"/>
+      <c r="X83" s="4"/>
+      <c r="Y83" s="4"/>
+      <c r="Z83" s="4"/>
+      <c r="AA83" s="4"/>
+    </row>
+    <row r="84" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+      <c r="U84" s="4"/>
+      <c r="V84" s="4"/>
+      <c r="W84" s="4"/>
+      <c r="X84" s="4"/>
+      <c r="Y84" s="4"/>
+      <c r="Z84" s="4"/>
+      <c r="AA84" s="4"/>
+    </row>
+    <row r="85" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="4"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+      <c r="U85" s="4"/>
+      <c r="V85" s="4"/>
+      <c r="W85" s="4"/>
+      <c r="X85" s="4"/>
+      <c r="Y85" s="4"/>
+      <c r="Z85" s="4"/>
+      <c r="AA85" s="4"/>
+    </row>
+    <row r="86" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+      <c r="U86" s="4"/>
+      <c r="V86" s="4"/>
+      <c r="W86" s="4"/>
+      <c r="X86" s="4"/>
+      <c r="Y86" s="4"/>
+      <c r="Z86" s="4"/>
+      <c r="AA86" s="4"/>
+    </row>
+    <row r="87" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="4"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+      <c r="U87" s="4"/>
+      <c r="V87" s="4"/>
+      <c r="W87" s="4"/>
+      <c r="X87" s="4"/>
+      <c r="Y87" s="4"/>
+      <c r="Z87" s="4"/>
+      <c r="AA87" s="4"/>
+    </row>
+    <row r="88" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+      <c r="U88" s="4"/>
+      <c r="V88" s="4"/>
+      <c r="W88" s="4"/>
+      <c r="X88" s="4"/>
+      <c r="Y88" s="4"/>
+      <c r="Z88" s="4"/>
+      <c r="AA88" s="4"/>
+    </row>
+    <row r="89" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
+      <c r="Y89" s="4"/>
+      <c r="Z89" s="4"/>
+      <c r="AA89" s="4"/>
+    </row>
+    <row r="90" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+      <c r="U90" s="4"/>
+      <c r="V90" s="4"/>
+      <c r="W90" s="4"/>
+      <c r="X90" s="4"/>
+      <c r="Y90" s="4"/>
+      <c r="Z90" s="4"/>
+      <c r="AA90" s="4"/>
+    </row>
+    <row r="91" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="4"/>
+      <c r="S91" s="4"/>
+      <c r="T91" s="4"/>
+      <c r="U91" s="4"/>
+      <c r="V91" s="4"/>
+      <c r="W91" s="4"/>
+      <c r="X91" s="4"/>
+      <c r="Y91" s="4"/>
+      <c r="Z91" s="4"/>
+      <c r="AA91" s="4"/>
+    </row>
+    <row r="92" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="4"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+      <c r="U92" s="4"/>
+      <c r="V92" s="4"/>
+      <c r="W92" s="4"/>
+      <c r="X92" s="4"/>
+      <c r="Y92" s="4"/>
+      <c r="Z92" s="4"/>
+      <c r="AA92" s="4"/>
+    </row>
+    <row r="93" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="4"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+      <c r="U93" s="4"/>
+      <c r="V93" s="4"/>
+      <c r="W93" s="4"/>
+      <c r="X93" s="4"/>
+      <c r="Y93" s="4"/>
+      <c r="Z93" s="4"/>
+      <c r="AA93" s="4"/>
+    </row>
+    <row r="94" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+      <c r="U94" s="4"/>
+      <c r="V94" s="4"/>
+      <c r="W94" s="4"/>
+      <c r="X94" s="4"/>
+      <c r="Y94" s="4"/>
+      <c r="Z94" s="4"/>
+      <c r="AA94" s="4"/>
+    </row>
+    <row r="95" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
+      <c r="S95" s="4"/>
+      <c r="T95" s="4"/>
+      <c r="U95" s="4"/>
+      <c r="V95" s="4"/>
+      <c r="W95" s="4"/>
+      <c r="X95" s="4"/>
+      <c r="Y95" s="4"/>
+      <c r="Z95" s="4"/>
+      <c r="AA95" s="4"/>
+    </row>
+    <row r="96" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B96" s="4"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+      <c r="U96" s="4"/>
+      <c r="V96" s="4"/>
+      <c r="W96" s="4"/>
+      <c r="X96" s="4"/>
+      <c r="Y96" s="4"/>
+      <c r="Z96" s="4"/>
+      <c r="AA96" s="4"/>
+    </row>
+    <row r="97" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B97" s="4"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+      <c r="U97" s="4"/>
+      <c r="V97" s="4"/>
+      <c r="W97" s="4"/>
+      <c r="X97" s="4"/>
+      <c r="Y97" s="4"/>
+      <c r="Z97" s="4"/>
+      <c r="AA97" s="4"/>
+    </row>
+    <row r="98" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="4"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+      <c r="U98" s="4"/>
+      <c r="V98" s="4"/>
+      <c r="W98" s="4"/>
+      <c r="X98" s="4"/>
+      <c r="Y98" s="4"/>
+      <c r="Z98" s="4"/>
+      <c r="AA98" s="4"/>
+    </row>
+    <row r="99" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="4"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+      <c r="U99" s="4"/>
+      <c r="V99" s="4"/>
+      <c r="W99" s="4"/>
+      <c r="X99" s="4"/>
+      <c r="Y99" s="4"/>
+      <c r="Z99" s="4"/>
+      <c r="AA99" s="4"/>
+    </row>
+    <row r="100" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="4"/>
+      <c r="S100" s="4"/>
+      <c r="T100" s="4"/>
+      <c r="U100" s="4"/>
+      <c r="V100" s="4"/>
+      <c r="W100" s="4"/>
+      <c r="X100" s="4"/>
+      <c r="Y100" s="4"/>
+      <c r="Z100" s="4"/>
+      <c r="AA100" s="4"/>
+    </row>
+    <row r="101" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B101" s="4"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="4"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+      <c r="U101" s="4"/>
+      <c r="V101" s="4"/>
+      <c r="W101" s="4"/>
+      <c r="X101" s="4"/>
+      <c r="Y101" s="4"/>
+      <c r="Z101" s="4"/>
+      <c r="AA101" s="4"/>
+    </row>
+    <row r="102" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B102" s="4"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="4"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+      <c r="U102" s="4"/>
+      <c r="V102" s="4"/>
+      <c r="W102" s="4"/>
+      <c r="X102" s="4"/>
+      <c r="Y102" s="4"/>
+      <c r="Z102" s="4"/>
+      <c r="AA102" s="4"/>
+    </row>
+    <row r="103" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B103" s="4"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="4"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+      <c r="U103" s="4"/>
+      <c r="V103" s="4"/>
+      <c r="W103" s="4"/>
+      <c r="X103" s="4"/>
+      <c r="Y103" s="4"/>
+      <c r="Z103" s="4"/>
+      <c r="AA103" s="4"/>
+    </row>
+    <row r="104" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+      <c r="U104" s="4"/>
+      <c r="V104" s="4"/>
+      <c r="W104" s="4"/>
+      <c r="X104" s="4"/>
+      <c r="Y104" s="4"/>
+      <c r="Z104" s="4"/>
+      <c r="AA104" s="4"/>
+    </row>
+    <row r="105" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B105" s="4"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+      <c r="U105" s="4"/>
+      <c r="V105" s="4"/>
+      <c r="W105" s="4"/>
+      <c r="X105" s="4"/>
+      <c r="Y105" s="4"/>
+      <c r="Z105" s="4"/>
+      <c r="AA105" s="4"/>
+    </row>
+    <row r="106" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B106" s="4"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="4"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+      <c r="U106" s="4"/>
+      <c r="V106" s="4"/>
+      <c r="W106" s="4"/>
+      <c r="X106" s="4"/>
+      <c r="Y106" s="4"/>
+      <c r="Z106" s="4"/>
+      <c r="AA106" s="4"/>
+    </row>
+    <row r="107" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B107" s="4"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+      <c r="V107" s="4"/>
+      <c r="W107" s="4"/>
+      <c r="X107" s="4"/>
+      <c r="Y107" s="4"/>
+      <c r="Z107" s="4"/>
+      <c r="AA107" s="4"/>
+    </row>
+    <row r="108" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B108" s="4"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="4"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+      <c r="U108" s="4"/>
+      <c r="V108" s="4"/>
+      <c r="W108" s="4"/>
+      <c r="X108" s="4"/>
+      <c r="Y108" s="4"/>
+      <c r="Z108" s="4"/>
+      <c r="AA108" s="4"/>
+    </row>
+    <row r="109" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B109" s="4"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="4"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+      <c r="U109" s="4"/>
+      <c r="V109" s="4"/>
+      <c r="W109" s="4"/>
+      <c r="X109" s="4"/>
+      <c r="Y109" s="4"/>
+      <c r="Z109" s="4"/>
+      <c r="AA109" s="4"/>
+    </row>
+    <row r="110" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B110" s="4"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="4"/>
+      <c r="S110" s="4"/>
+      <c r="T110" s="4"/>
+      <c r="U110" s="4"/>
+      <c r="V110" s="4"/>
+      <c r="W110" s="4"/>
+      <c r="X110" s="4"/>
+      <c r="Y110" s="4"/>
+      <c r="Z110" s="4"/>
+      <c r="AA110" s="4"/>
+    </row>
+    <row r="111" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4"/>
+      <c r="V111" s="4"/>
+      <c r="W111" s="4"/>
+      <c r="X111" s="4"/>
+      <c r="Y111" s="4"/>
+      <c r="Z111" s="4"/>
+      <c r="AA111" s="4"/>
+    </row>
+    <row r="112" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+      <c r="U112" s="4"/>
+      <c r="V112" s="4"/>
+      <c r="W112" s="4"/>
+      <c r="X112" s="4"/>
+      <c r="Y112" s="4"/>
+      <c r="Z112" s="4"/>
+      <c r="AA112" s="4"/>
+    </row>
+    <row r="113" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="4"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4"/>
+      <c r="U113" s="4"/>
+      <c r="V113" s="4"/>
+      <c r="W113" s="4"/>
+      <c r="X113" s="4"/>
+      <c r="Y113" s="4"/>
+      <c r="Z113" s="4"/>
+      <c r="AA113" s="4"/>
+    </row>
+    <row r="114" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4"/>
+      <c r="W114" s="4"/>
+      <c r="X114" s="4"/>
+      <c r="Y114" s="4"/>
+      <c r="Z114" s="4"/>
+      <c r="AA114" s="4"/>
+    </row>
+    <row r="115" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="4"/>
+      <c r="W115" s="4"/>
+      <c r="X115" s="4"/>
+      <c r="Y115" s="4"/>
+      <c r="Z115" s="4"/>
+      <c r="AA115" s="4"/>
+    </row>
+    <row r="116" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
+      <c r="L116" s="4"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="4"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+      <c r="U116" s="4"/>
+      <c r="V116" s="4"/>
+      <c r="W116" s="4"/>
+      <c r="X116" s="4"/>
+      <c r="Y116" s="4"/>
+      <c r="Z116" s="4"/>
+      <c r="AA116" s="4"/>
+    </row>
+    <row r="117" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="4"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+      <c r="U117" s="4"/>
+      <c r="V117" s="4"/>
+      <c r="W117" s="4"/>
+      <c r="X117" s="4"/>
+      <c r="Y117" s="4"/>
+      <c r="Z117" s="4"/>
+      <c r="AA117" s="4"/>
+    </row>
+    <row r="118" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
+      <c r="X118" s="4"/>
+      <c r="Y118" s="4"/>
+      <c r="Z118" s="4"/>
+      <c r="AA118" s="4"/>
+    </row>
+    <row r="119" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B119" s="4"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="4"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+      <c r="U119" s="4"/>
+      <c r="V119" s="4"/>
+      <c r="W119" s="4"/>
+      <c r="X119" s="4"/>
+      <c r="Y119" s="4"/>
+      <c r="Z119" s="4"/>
+      <c r="AA119" s="4"/>
+    </row>
+    <row r="120" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="4"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+      <c r="U120" s="4"/>
+      <c r="V120" s="4"/>
+      <c r="W120" s="4"/>
+      <c r="X120" s="4"/>
+      <c r="Y120" s="4"/>
+      <c r="Z120" s="4"/>
+      <c r="AA120" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9285E49-3904-41E2-8BC2-2CD7AA16ED58}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AA120"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.19921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.69921875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.69921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.69921875" style="3" customWidth="1"/>
+    <col min="7" max="11" width="10.69921875" style="3"/>
+    <col min="12" max="12" width="1.69921875" style="3" customWidth="1"/>
+    <col min="13" max="19" width="10.69921875" style="3"/>
+    <col min="20" max="20" width="10.69921875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10.69921875" style="3"/>
+    <col min="22" max="22" width="3.19921875" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="10.69921875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="2:27" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+    </row>
+    <row r="3" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+    </row>
+    <row r="4" spans="2:27" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+    </row>
+    <row r="5" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9">
+        <v>6</v>
+      </c>
+      <c r="I5" s="9">
+        <v>6</v>
+      </c>
+      <c r="J5" s="9">
+        <v>6</v>
+      </c>
+      <c r="K5" s="9">
+        <v>6</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+    </row>
+    <row r="6" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5</v>
+      </c>
+      <c r="G6" s="9">
+        <v>5</v>
+      </c>
+      <c r="H6" s="9">
+        <v>5</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+    </row>
+    <row r="7" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="9">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+    </row>
+    <row r="8" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+    </row>
+    <row r="9" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9">
+        <v>10</v>
+      </c>
+      <c r="H9" s="9">
+        <v>5</v>
+      </c>
+      <c r="I9" s="9">
+        <v>3</v>
+      </c>
+      <c r="J9" s="9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+    </row>
+    <row r="10" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="9">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
+      <c r="H10" s="9">
+        <v>5</v>
+      </c>
+      <c r="I10" s="9">
+        <v>3</v>
+      </c>
+      <c r="J10" s="9">
+        <v>2</v>
+      </c>
+      <c r="K10" s="9">
+        <v>2</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+    </row>
+    <row r="11" spans="2:27" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+    </row>
+    <row r="12" spans="2:27" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9">
+        <v>3</v>
+      </c>
+      <c r="G12" s="9">
+        <v>3</v>
+      </c>
+      <c r="H12" s="9">
+        <v>3</v>
+      </c>
+      <c r="I12" s="9">
+        <v>3</v>
+      </c>
+      <c r="J12" s="9">
+        <v>3</v>
+      </c>
+      <c r="K12" s="9">
+        <v>3</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3</v>
+      </c>
+      <c r="H13" s="9">
+        <v>3</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+    </row>
+    <row r="14" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+    </row>
+    <row r="15" spans="2:27" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="9">
+        <v>5</v>
+      </c>
+      <c r="G15" s="9">
+        <v>5</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+    </row>
+    <row r="16" spans="2:27" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="9">
+        <v>4</v>
+      </c>
+      <c r="G16" s="9">
+        <v>4</v>
+      </c>
+      <c r="H16" s="9">
+        <v>2</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="9">
+        <v>8</v>
+      </c>
+      <c r="G17" s="9">
+        <v>8</v>
+      </c>
+      <c r="H17" s="9">
+        <v>8</v>
+      </c>
+      <c r="I17" s="9">
+        <v>4</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+    </row>
+    <row r="18" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+    </row>
+    <row r="19" spans="2:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="9">
+        <v>10</v>
+      </c>
+      <c r="G19" s="9">
+        <v>7</v>
+      </c>
+      <c r="H19" s="9">
+        <v>5</v>
+      </c>
+      <c r="I19" s="9">
+        <v>3</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+    </row>
+    <row r="20" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+    </row>
+    <row r="21" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="9">
+        <v>4</v>
+      </c>
+      <c r="G21" s="9">
+        <v>4</v>
+      </c>
+      <c r="H21" s="9">
+        <v>2</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+    </row>
+    <row r="22" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="9">
+        <v>2</v>
+      </c>
+      <c r="G22" s="9">
+        <v>2</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+    </row>
+    <row r="23" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="9">
+        <v>2</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2</v>
+      </c>
+      <c r="H23" s="9">
+        <v>2</v>
+      </c>
+      <c r="I23" s="9">
+        <v>2</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+    </row>
+    <row r="24" spans="2:27" s="10" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2</v>
+      </c>
+      <c r="H24" s="9">
+        <v>2</v>
+      </c>
+      <c r="I24" s="9">
+        <v>2</v>
+      </c>
+      <c r="J24" s="9">
+        <v>1</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+    </row>
+    <row r="25" spans="2:27" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5">
+        <f>SUM(F3:F24)</f>
+        <v>89</v>
+      </c>
+      <c r="G25" s="5">
+        <f>SUM(G3:G24)</f>
+        <v>76</v>
+      </c>
+      <c r="H25" s="5">
+        <f>SUM(H3:H24)</f>
+        <v>55</v>
+      </c>
+      <c r="I25" s="5">
+        <f>SUM(I3:I24)</f>
+        <v>38</v>
+      </c>
+      <c r="J25" s="5">
+        <f>SUM(J3:J24)</f>
+        <v>15</v>
+      </c>
+      <c r="K25" s="5">
+        <f>SUM(K3:K24)</f>
+        <v>13</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>

</xml_diff>